<commit_message>
hunger games data done
</commit_message>
<xml_diff>
--- a/4-childrens-series/hunger-games.xlsx
+++ b/4-childrens-series/hunger-games.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsayhuth/Documents/GitHub/movies-and-their-books/4-childrens-series/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/4-childrens-series/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06A7DEF-193A-7A45-B64E-51C494CD6927}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{786464B7-A673-ED4E-AD4C-AFA1EC79B351}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="16840" windowHeight="16400" xr2:uid="{AC7901C7-1EE3-AA47-BDC0-FCB01F27881B}"/>
+    <workbookView xWindow="30640" yWindow="2500" windowWidth="20700" windowHeight="21180" xr2:uid="{AC7901C7-1EE3-AA47-BDC0-FCB01F27881B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="12">
   <si>
     <t>Published Date</t>
   </si>
@@ -39,7 +39,28 @@
     <t>Bestsellers Date</t>
   </si>
   <si>
-    <t>start with 43.json</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>First Opens: 2012-03-23</t>
+  </si>
+  <si>
+    <t>First Closes: 2012-09-06</t>
+  </si>
+  <si>
+    <t>Second Opens: 2013-11-22</t>
+  </si>
+  <si>
+    <t>Second Closes: 2013-04-03</t>
+  </si>
+  <si>
+    <t>Third Opens: 2014-11-21</t>
+  </si>
+  <si>
+    <t>Third Closes: 2015-03-19</t>
+  </si>
+  <si>
+    <t>Fourth Opens: 2015-11-20</t>
   </si>
 </sst>
 </file>
@@ -58,12 +79,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,11 +111,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,16 +434,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E2E8DD-A8F5-4740-B8E8-9F99CB838420}">
-  <dimension ref="A1:E256"/>
+  <dimension ref="A1:E278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1653,343 +1691,394 @@
         <v>40985</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="2">
+    <row r="84" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
         <v>41007</v>
       </c>
-      <c r="B84" s="3">
-        <v>1</v>
-      </c>
-      <c r="C84" s="3">
-        <v>10</v>
-      </c>
-      <c r="D84" s="2">
+      <c r="B84" s="5">
+        <v>1</v>
+      </c>
+      <c r="C84" s="5">
+        <v>10</v>
+      </c>
+      <c r="D84" s="4">
         <f t="shared" si="1"/>
         <v>40992</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="2">
+      <c r="E84" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
         <v>41014</v>
       </c>
-      <c r="B85" s="3">
-        <v>1</v>
-      </c>
-      <c r="C85" s="3">
-        <v>10</v>
-      </c>
-      <c r="D85" s="2">
+      <c r="B85" s="7">
+        <v>1</v>
+      </c>
+      <c r="C85" s="7">
+        <v>10</v>
+      </c>
+      <c r="D85" s="6">
         <f t="shared" si="1"/>
         <v>40999</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="2">
+    <row r="86" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
         <v>41021</v>
       </c>
-      <c r="B86" s="3">
-        <v>1</v>
-      </c>
-      <c r="C86" s="3">
-        <v>10</v>
-      </c>
-      <c r="D86" s="2">
+      <c r="B86" s="7">
+        <v>1</v>
+      </c>
+      <c r="C86" s="7">
+        <v>10</v>
+      </c>
+      <c r="D86" s="6">
         <f t="shared" si="1"/>
         <v>41006</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="2">
+    <row r="87" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
         <v>41028</v>
       </c>
-      <c r="B87" s="3">
-        <v>1</v>
-      </c>
-      <c r="C87" s="3">
-        <v>10</v>
-      </c>
-      <c r="D87" s="2">
+      <c r="B87" s="7">
+        <v>1</v>
+      </c>
+      <c r="C87" s="7">
+        <v>10</v>
+      </c>
+      <c r="D87" s="6">
         <f t="shared" si="1"/>
         <v>41013</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2">
+    <row r="88" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
         <v>41035</v>
       </c>
-      <c r="B88" s="3">
-        <v>1</v>
-      </c>
-      <c r="C88" s="3">
-        <v>10</v>
-      </c>
-      <c r="D88" s="2">
+      <c r="B88" s="7">
+        <v>1</v>
+      </c>
+      <c r="C88" s="7">
+        <v>10</v>
+      </c>
+      <c r="D88" s="6">
         <f t="shared" si="1"/>
         <v>41020</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="2">
+    <row r="89" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
         <v>41042</v>
       </c>
-      <c r="B89" s="3">
-        <v>1</v>
-      </c>
-      <c r="C89" s="3">
-        <v>10</v>
-      </c>
-      <c r="D89" s="2">
+      <c r="B89" s="7">
+        <v>1</v>
+      </c>
+      <c r="C89" s="7">
+        <v>10</v>
+      </c>
+      <c r="D89" s="6">
         <f t="shared" si="1"/>
         <v>41027</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="2">
+    <row r="90" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
         <v>41049</v>
       </c>
-      <c r="B90" s="3">
-        <v>1</v>
-      </c>
-      <c r="C90" s="3">
-        <v>10</v>
-      </c>
-      <c r="D90" s="2">
+      <c r="B90" s="7">
+        <v>1</v>
+      </c>
+      <c r="C90" s="7">
+        <v>10</v>
+      </c>
+      <c r="D90" s="6">
         <f t="shared" ref="D90:D153" si="2">A90-15</f>
         <v>41034</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="2">
+    <row r="91" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
         <v>41056</v>
       </c>
-      <c r="B91" s="3">
-        <v>1</v>
-      </c>
-      <c r="C91" s="3">
-        <v>10</v>
-      </c>
-      <c r="D91" s="2">
+      <c r="B91" s="7">
+        <v>1</v>
+      </c>
+      <c r="C91" s="7">
+        <v>10</v>
+      </c>
+      <c r="D91" s="6">
         <f t="shared" si="2"/>
         <v>41041</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="2">
+    <row r="92" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
         <v>41063</v>
       </c>
-      <c r="B92" s="3">
-        <v>1</v>
-      </c>
-      <c r="C92" s="3">
-        <v>10</v>
-      </c>
-      <c r="D92" s="2">
+      <c r="B92" s="7">
+        <v>1</v>
+      </c>
+      <c r="C92" s="7">
+        <v>10</v>
+      </c>
+      <c r="D92" s="6">
         <f t="shared" si="2"/>
         <v>41048</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="2">
+    <row r="93" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
         <v>41070</v>
       </c>
-      <c r="B93" s="3">
-        <v>1</v>
-      </c>
-      <c r="C93" s="3">
-        <v>10</v>
-      </c>
-      <c r="D93" s="2">
+      <c r="B93" s="7">
+        <v>1</v>
+      </c>
+      <c r="C93" s="7">
+        <v>10</v>
+      </c>
+      <c r="D93" s="6">
         <f t="shared" si="2"/>
         <v>41055</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="2">
+    <row r="94" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
         <v>41077</v>
       </c>
-      <c r="C94" s="3">
-        <v>10</v>
-      </c>
-      <c r="D94" s="2">
+      <c r="B94" s="7">
+        <v>1</v>
+      </c>
+      <c r="C94" s="7">
+        <v>10</v>
+      </c>
+      <c r="D94" s="6">
         <f t="shared" si="2"/>
         <v>41062</v>
       </c>
-      <c r="E94" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="2">
+    </row>
+    <row r="95" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
         <v>41084</v>
       </c>
-      <c r="C95" s="3">
-        <v>10</v>
-      </c>
-      <c r="D95" s="2">
+      <c r="B95" s="7">
+        <v>1</v>
+      </c>
+      <c r="C95" s="7">
+        <v>10</v>
+      </c>
+      <c r="D95" s="6">
         <f t="shared" si="2"/>
         <v>41069</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="2">
+    <row r="96" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
         <v>41091</v>
       </c>
-      <c r="C96" s="3">
-        <v>10</v>
-      </c>
-      <c r="D96" s="2">
+      <c r="B96" s="7">
+        <v>1</v>
+      </c>
+      <c r="C96" s="7">
+        <v>10</v>
+      </c>
+      <c r="D96" s="6">
         <f t="shared" si="2"/>
         <v>41076</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="2">
+    <row r="97" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
         <v>41098</v>
       </c>
-      <c r="C97" s="3">
-        <v>10</v>
-      </c>
-      <c r="D97" s="2">
+      <c r="B97" s="7">
+        <v>1</v>
+      </c>
+      <c r="C97" s="7">
+        <v>10</v>
+      </c>
+      <c r="D97" s="6">
         <f t="shared" si="2"/>
         <v>41083</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="2">
+    <row r="98" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
         <v>41105</v>
       </c>
-      <c r="C98" s="3">
-        <v>10</v>
-      </c>
-      <c r="D98" s="2">
+      <c r="B98" s="7">
+        <v>1</v>
+      </c>
+      <c r="C98" s="7">
+        <v>10</v>
+      </c>
+      <c r="D98" s="6">
         <f t="shared" si="2"/>
         <v>41090</v>
       </c>
     </row>
-    <row r="99" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="2">
+    <row r="99" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
         <v>41112</v>
       </c>
-      <c r="C99" s="3">
-        <v>10</v>
-      </c>
-      <c r="D99" s="2">
+      <c r="B99" s="7">
+        <v>1</v>
+      </c>
+      <c r="C99" s="7">
+        <v>10</v>
+      </c>
+      <c r="D99" s="6">
         <f t="shared" si="2"/>
         <v>41097</v>
       </c>
     </row>
-    <row r="100" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="2">
+    <row r="100" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
         <v>41119</v>
       </c>
-      <c r="C100" s="3">
-        <v>10</v>
-      </c>
-      <c r="D100" s="2">
+      <c r="B100" s="7">
+        <v>1</v>
+      </c>
+      <c r="C100" s="7">
+        <v>10</v>
+      </c>
+      <c r="D100" s="6">
         <f t="shared" si="2"/>
         <v>41104</v>
       </c>
     </row>
-    <row r="101" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="2">
+    <row r="101" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
         <v>41126</v>
       </c>
-      <c r="C101" s="3">
-        <v>10</v>
-      </c>
-      <c r="D101" s="2">
+      <c r="B101" s="7">
+        <v>1</v>
+      </c>
+      <c r="C101" s="7">
+        <v>10</v>
+      </c>
+      <c r="D101" s="6">
         <f t="shared" si="2"/>
         <v>41111</v>
       </c>
     </row>
-    <row r="102" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="2">
+    <row r="102" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
         <v>41133</v>
       </c>
-      <c r="C102" s="3">
-        <v>10</v>
-      </c>
-      <c r="D102" s="2">
+      <c r="B102" s="7">
+        <v>1</v>
+      </c>
+      <c r="C102" s="7">
+        <v>10</v>
+      </c>
+      <c r="D102" s="6">
         <f t="shared" si="2"/>
         <v>41118</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="2">
+    <row r="103" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="6">
         <v>41140</v>
       </c>
-      <c r="C103" s="3">
-        <v>10</v>
-      </c>
-      <c r="D103" s="2">
+      <c r="B103" s="7">
+        <v>1</v>
+      </c>
+      <c r="C103" s="7">
+        <v>10</v>
+      </c>
+      <c r="D103" s="6">
         <f t="shared" si="2"/>
         <v>41125</v>
       </c>
     </row>
-    <row r="104" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="2">
+    <row r="104" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="6">
         <v>41147</v>
       </c>
-      <c r="C104" s="3">
-        <v>10</v>
-      </c>
-      <c r="D104" s="2">
+      <c r="B104" s="7">
+        <v>1</v>
+      </c>
+      <c r="C104" s="7">
+        <v>10</v>
+      </c>
+      <c r="D104" s="6">
         <f t="shared" si="2"/>
         <v>41132</v>
       </c>
     </row>
-    <row r="105" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="2">
+    <row r="105" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
         <v>41154</v>
       </c>
-      <c r="C105" s="3">
-        <v>10</v>
-      </c>
-      <c r="D105" s="2">
+      <c r="B105" s="7">
+        <v>1</v>
+      </c>
+      <c r="C105" s="7">
+        <v>10</v>
+      </c>
+      <c r="D105" s="6">
         <f t="shared" si="2"/>
         <v>41139</v>
       </c>
     </row>
-    <row r="106" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="2">
+    <row r="106" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="6">
         <v>41161</v>
       </c>
-      <c r="C106" s="3">
-        <v>10</v>
-      </c>
-      <c r="D106" s="2">
+      <c r="B106" s="7">
+        <v>1</v>
+      </c>
+      <c r="C106" s="7">
+        <v>10</v>
+      </c>
+      <c r="D106" s="6">
         <f t="shared" si="2"/>
         <v>41146</v>
       </c>
     </row>
-    <row r="107" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="2">
+    <row r="107" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="6">
         <v>41168</v>
       </c>
-      <c r="C107" s="3">
-        <v>10</v>
-      </c>
-      <c r="D107" s="2">
+      <c r="B107" s="7">
+        <v>1</v>
+      </c>
+      <c r="C107" s="7">
+        <v>10</v>
+      </c>
+      <c r="D107" s="6">
         <f t="shared" si="2"/>
         <v>41153</v>
       </c>
     </row>
-    <row r="108" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="2">
+    <row r="108" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="4">
         <v>41175</v>
       </c>
-      <c r="C108" s="3">
-        <v>10</v>
-      </c>
-      <c r="D108" s="2">
+      <c r="B108" s="5">
+        <v>1</v>
+      </c>
+      <c r="C108" s="5">
+        <v>10</v>
+      </c>
+      <c r="D108" s="4">
         <f t="shared" si="2"/>
         <v>41160</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E108" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>41182</v>
       </c>
+      <c r="B109" s="3">
+        <v>1</v>
+      </c>
       <c r="C109" s="3">
         <v>10</v>
       </c>
@@ -1998,10 +2087,13 @@
         <v>41167</v>
       </c>
     </row>
-    <row r="110" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>41189</v>
       </c>
+      <c r="B110" s="3">
+        <v>1</v>
+      </c>
       <c r="C110" s="3">
         <v>10</v>
       </c>
@@ -2010,10 +2102,13 @@
         <v>41174</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>41196</v>
       </c>
+      <c r="B111" s="3">
+        <v>1</v>
+      </c>
       <c r="C111" s="3">
         <v>10</v>
       </c>
@@ -2022,9 +2117,12 @@
         <v>41181</v>
       </c>
     </row>
-    <row r="112" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>41203</v>
+      </c>
+      <c r="B112" s="3">
+        <v>2</v>
       </c>
       <c r="C112" s="3">
         <v>10</v>
@@ -2038,6 +2136,9 @@
       <c r="A113" s="2">
         <v>41210</v>
       </c>
+      <c r="B113" s="3">
+        <v>2</v>
+      </c>
       <c r="C113" s="3">
         <v>10</v>
       </c>
@@ -2050,6 +2151,9 @@
       <c r="A114" s="2">
         <v>41217</v>
       </c>
+      <c r="B114" s="3">
+        <v>2</v>
+      </c>
       <c r="C114" s="3">
         <v>10</v>
       </c>
@@ -2062,6 +2166,9 @@
       <c r="A115" s="2">
         <v>41224</v>
       </c>
+      <c r="B115" s="3">
+        <v>2</v>
+      </c>
       <c r="C115" s="3">
         <v>10</v>
       </c>
@@ -2074,6 +2181,9 @@
       <c r="A116" s="2">
         <v>41231</v>
       </c>
+      <c r="B116" s="3">
+        <v>2</v>
+      </c>
       <c r="C116" s="3">
         <v>10</v>
       </c>
@@ -2086,6 +2196,9 @@
       <c r="A117" s="2">
         <v>41238</v>
       </c>
+      <c r="B117" s="3">
+        <v>1</v>
+      </c>
       <c r="C117" s="3">
         <v>10</v>
       </c>
@@ -2098,6 +2211,9 @@
       <c r="A118" s="2">
         <v>41245</v>
       </c>
+      <c r="B118" s="3">
+        <v>4</v>
+      </c>
       <c r="C118" s="3">
         <v>10</v>
       </c>
@@ -2110,6 +2226,9 @@
       <c r="A119" s="2">
         <v>41252</v>
       </c>
+      <c r="B119" s="3">
+        <v>2</v>
+      </c>
       <c r="C119" s="3">
         <v>10</v>
       </c>
@@ -2122,6 +2241,9 @@
       <c r="A120" s="2">
         <v>41259</v>
       </c>
+      <c r="B120" s="3">
+        <v>2</v>
+      </c>
       <c r="C120" s="3">
         <v>10</v>
       </c>
@@ -2134,6 +2256,9 @@
       <c r="A121" s="2">
         <v>41266</v>
       </c>
+      <c r="B121" s="3">
+        <v>2</v>
+      </c>
       <c r="C121" s="3">
         <v>10</v>
       </c>
@@ -2146,6 +2271,9 @@
       <c r="A122" s="2">
         <v>41273</v>
       </c>
+      <c r="B122" s="3">
+        <v>2</v>
+      </c>
       <c r="C122" s="3">
         <v>10</v>
       </c>
@@ -2158,6 +2286,9 @@
       <c r="A123" s="2">
         <v>41280</v>
       </c>
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
       <c r="C123" s="3">
         <v>10</v>
       </c>
@@ -2170,6 +2301,9 @@
       <c r="A124" s="2">
         <v>41287</v>
       </c>
+      <c r="B124" s="3">
+        <v>2</v>
+      </c>
       <c r="C124" s="3">
         <v>10</v>
       </c>
@@ -2182,6 +2316,9 @@
       <c r="A125" s="2">
         <v>41294</v>
       </c>
+      <c r="B125" s="3">
+        <v>1</v>
+      </c>
       <c r="C125" s="3">
         <v>10</v>
       </c>
@@ -2194,6 +2331,9 @@
       <c r="A126" s="2">
         <v>41301</v>
       </c>
+      <c r="B126" s="3">
+        <v>1</v>
+      </c>
       <c r="C126" s="3">
         <v>10</v>
       </c>
@@ -2206,6 +2346,9 @@
       <c r="A127" s="2">
         <v>41308</v>
       </c>
+      <c r="B127" s="3">
+        <v>1</v>
+      </c>
       <c r="C127" s="3">
         <v>10</v>
       </c>
@@ -2218,6 +2361,9 @@
       <c r="A128" s="2">
         <v>41315</v>
       </c>
+      <c r="B128" s="3">
+        <v>1</v>
+      </c>
       <c r="C128" s="3">
         <v>10</v>
       </c>
@@ -2230,6 +2376,9 @@
       <c r="A129" s="2">
         <v>41322</v>
       </c>
+      <c r="B129" s="3">
+        <v>1</v>
+      </c>
       <c r="C129" s="3">
         <v>10</v>
       </c>
@@ -2242,6 +2391,9 @@
       <c r="A130" s="2">
         <v>41329</v>
       </c>
+      <c r="B130" s="3">
+        <v>2</v>
+      </c>
       <c r="C130" s="3">
         <v>10</v>
       </c>
@@ -2254,6 +2406,9 @@
       <c r="A131" s="2">
         <v>41336</v>
       </c>
+      <c r="B131" s="3">
+        <v>3</v>
+      </c>
       <c r="C131" s="3">
         <v>10</v>
       </c>
@@ -2266,6 +2421,9 @@
       <c r="A132" s="2">
         <v>41343</v>
       </c>
+      <c r="B132" s="3">
+        <v>2</v>
+      </c>
       <c r="C132" s="3">
         <v>10</v>
       </c>
@@ -2278,6 +2436,9 @@
       <c r="A133" s="2">
         <v>41350</v>
       </c>
+      <c r="B133" s="3">
+        <v>2</v>
+      </c>
       <c r="C133" s="3">
         <v>10</v>
       </c>
@@ -2290,6 +2451,9 @@
       <c r="A134" s="2">
         <v>41357</v>
       </c>
+      <c r="B134" s="3">
+        <v>1</v>
+      </c>
       <c r="C134" s="3">
         <v>10</v>
       </c>
@@ -2302,6 +2466,9 @@
       <c r="A135" s="2">
         <v>41364</v>
       </c>
+      <c r="B135" s="3">
+        <v>1</v>
+      </c>
       <c r="C135" s="3">
         <v>10</v>
       </c>
@@ -2314,6 +2481,9 @@
       <c r="A136" s="2">
         <v>41371</v>
       </c>
+      <c r="B136" s="3">
+        <v>2</v>
+      </c>
       <c r="C136">
         <v>10</v>
       </c>
@@ -2326,6 +2496,9 @@
       <c r="A137" s="2">
         <v>41378</v>
       </c>
+      <c r="B137" s="3">
+        <v>3</v>
+      </c>
       <c r="C137">
         <v>10</v>
       </c>
@@ -2338,6 +2511,9 @@
       <c r="A138" s="2">
         <v>41385</v>
       </c>
+      <c r="B138" s="3">
+        <v>1</v>
+      </c>
       <c r="C138">
         <v>10</v>
       </c>
@@ -2350,6 +2526,9 @@
       <c r="A139" s="2">
         <v>41392</v>
       </c>
+      <c r="B139" s="3">
+        <v>1</v>
+      </c>
       <c r="C139">
         <v>10</v>
       </c>
@@ -2362,6 +2541,9 @@
       <c r="A140" s="2">
         <v>41399</v>
       </c>
+      <c r="B140" s="3">
+        <v>1</v>
+      </c>
       <c r="C140">
         <v>10</v>
       </c>
@@ -2374,6 +2556,9 @@
       <c r="A141" s="2">
         <v>41406</v>
       </c>
+      <c r="B141" s="3">
+        <v>1</v>
+      </c>
       <c r="C141">
         <v>10</v>
       </c>
@@ -2386,6 +2571,9 @@
       <c r="A142" s="2">
         <v>41413</v>
       </c>
+      <c r="B142" s="3">
+        <v>1</v>
+      </c>
       <c r="C142">
         <v>10</v>
       </c>
@@ -2398,6 +2586,9 @@
       <c r="A143" s="2">
         <v>41420</v>
       </c>
+      <c r="B143" s="3">
+        <v>1</v>
+      </c>
       <c r="C143">
         <v>10</v>
       </c>
@@ -2410,6 +2601,9 @@
       <c r="A144" s="2">
         <v>41427</v>
       </c>
+      <c r="B144" s="3">
+        <v>1</v>
+      </c>
       <c r="C144">
         <v>10</v>
       </c>
@@ -2422,6 +2616,9 @@
       <c r="A145" s="2">
         <v>41434</v>
       </c>
+      <c r="B145" s="3">
+        <v>1</v>
+      </c>
       <c r="C145">
         <v>10</v>
       </c>
@@ -2434,6 +2631,9 @@
       <c r="A146" s="2">
         <v>41441</v>
       </c>
+      <c r="B146" s="3">
+        <v>1</v>
+      </c>
       <c r="C146">
         <v>10</v>
       </c>
@@ -2446,6 +2646,9 @@
       <c r="A147" s="2">
         <v>41448</v>
       </c>
+      <c r="B147" s="3">
+        <v>2</v>
+      </c>
       <c r="C147">
         <v>10</v>
       </c>
@@ -2458,6 +2661,9 @@
       <c r="A148" s="2">
         <v>41455</v>
       </c>
+      <c r="B148" s="3">
+        <v>1</v>
+      </c>
       <c r="C148">
         <v>10</v>
       </c>
@@ -2470,6 +2676,9 @@
       <c r="A149" s="2">
         <v>41462</v>
       </c>
+      <c r="B149" s="3">
+        <v>1</v>
+      </c>
       <c r="C149">
         <v>10</v>
       </c>
@@ -2482,6 +2691,9 @@
       <c r="A150" s="2">
         <v>41469</v>
       </c>
+      <c r="B150" s="3">
+        <v>2</v>
+      </c>
       <c r="C150">
         <v>10</v>
       </c>
@@ -2494,6 +2706,9 @@
       <c r="A151" s="2">
         <v>41476</v>
       </c>
+      <c r="B151" s="3">
+        <v>2</v>
+      </c>
       <c r="C151">
         <v>10</v>
       </c>
@@ -2506,6 +2721,9 @@
       <c r="A152" s="2">
         <v>41483</v>
       </c>
+      <c r="B152" s="3">
+        <v>2</v>
+      </c>
       <c r="C152">
         <v>10</v>
       </c>
@@ -2518,6 +2736,9 @@
       <c r="A153" s="2">
         <v>41490</v>
       </c>
+      <c r="B153" s="3">
+        <v>2</v>
+      </c>
       <c r="C153">
         <v>10</v>
       </c>
@@ -2530,6 +2751,9 @@
       <c r="A154" s="2">
         <v>41497</v>
       </c>
+      <c r="B154" s="3">
+        <v>2</v>
+      </c>
       <c r="C154">
         <v>10</v>
       </c>
@@ -2542,6 +2766,9 @@
       <c r="A155" s="2">
         <v>41504</v>
       </c>
+      <c r="B155" s="3">
+        <v>2</v>
+      </c>
       <c r="C155">
         <v>10</v>
       </c>
@@ -2554,6 +2781,9 @@
       <c r="A156" s="2">
         <v>41511</v>
       </c>
+      <c r="B156" s="3">
+        <v>3</v>
+      </c>
       <c r="C156">
         <v>10</v>
       </c>
@@ -2566,6 +2796,9 @@
       <c r="A157" s="2">
         <v>41518</v>
       </c>
+      <c r="B157" s="3">
+        <v>3</v>
+      </c>
       <c r="C157">
         <v>10</v>
       </c>
@@ -2578,6 +2811,9 @@
       <c r="A158" s="2">
         <v>41525</v>
       </c>
+      <c r="B158" s="3">
+        <v>3</v>
+      </c>
       <c r="C158">
         <v>10</v>
       </c>
@@ -2590,6 +2826,9 @@
       <c r="A159" s="2">
         <v>41532</v>
       </c>
+      <c r="B159" s="3">
+        <v>3</v>
+      </c>
       <c r="C159">
         <v>10</v>
       </c>
@@ -2602,6 +2841,9 @@
       <c r="A160" s="2">
         <v>41539</v>
       </c>
+      <c r="B160" s="3">
+        <v>2</v>
+      </c>
       <c r="C160">
         <v>10</v>
       </c>
@@ -2610,10 +2852,13 @@
         <v>41524</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>41546</v>
       </c>
+      <c r="B161" s="3">
+        <v>2</v>
+      </c>
       <c r="C161">
         <v>10</v>
       </c>
@@ -2622,10 +2867,13 @@
         <v>41531</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>41553</v>
       </c>
+      <c r="B162" s="3">
+        <v>3</v>
+      </c>
       <c r="C162">
         <v>10</v>
       </c>
@@ -2634,10 +2882,13 @@
         <v>41538</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>41560</v>
       </c>
+      <c r="B163" s="3">
+        <v>2</v>
+      </c>
       <c r="C163">
         <v>10</v>
       </c>
@@ -2646,10 +2897,13 @@
         <v>41545</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>41567</v>
       </c>
+      <c r="B164" s="3">
+        <v>2</v>
+      </c>
       <c r="C164">
         <v>10</v>
       </c>
@@ -2658,10 +2912,13 @@
         <v>41552</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>41574</v>
       </c>
+      <c r="B165" s="3">
+        <v>3</v>
+      </c>
       <c r="C165">
         <v>10</v>
       </c>
@@ -2670,10 +2927,13 @@
         <v>41559</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>41581</v>
       </c>
+      <c r="B166" s="3">
+        <v>3</v>
+      </c>
       <c r="C166">
         <v>10</v>
       </c>
@@ -2682,10 +2942,13 @@
         <v>41566</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>41588</v>
       </c>
+      <c r="B167" s="3">
+        <v>4</v>
+      </c>
       <c r="C167">
         <v>10</v>
       </c>
@@ -2694,10 +2957,13 @@
         <v>41573</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>41595</v>
       </c>
+      <c r="B168" s="3">
+        <v>3</v>
+      </c>
       <c r="C168">
         <v>10</v>
       </c>
@@ -2706,10 +2972,13 @@
         <v>41580</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>41602</v>
       </c>
+      <c r="B169" s="3">
+        <v>4</v>
+      </c>
       <c r="C169">
         <v>10</v>
       </c>
@@ -2718,10 +2987,13 @@
         <v>41587</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>41609</v>
       </c>
+      <c r="B170" s="3">
+        <v>3</v>
+      </c>
       <c r="C170">
         <v>10</v>
       </c>
@@ -2730,250 +3002,319 @@
         <v>41594</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" s="2">
+    <row r="171" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="4">
         <v>41616</v>
       </c>
-      <c r="C171">
-        <v>10</v>
-      </c>
-      <c r="D171" s="1">
+      <c r="B171" s="5">
+        <v>3</v>
+      </c>
+      <c r="C171" s="5">
+        <v>10</v>
+      </c>
+      <c r="D171" s="4">
         <f t="shared" si="3"/>
         <v>41601</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" s="2">
+      <c r="E171" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="6">
         <v>41623</v>
       </c>
-      <c r="C172">
-        <v>10</v>
-      </c>
-      <c r="D172" s="1">
+      <c r="B172" s="7">
+        <v>2</v>
+      </c>
+      <c r="C172" s="7">
+        <v>10</v>
+      </c>
+      <c r="D172" s="6">
         <f t="shared" si="3"/>
         <v>41608</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" s="2">
+    <row r="173" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="6">
         <v>41630</v>
       </c>
-      <c r="C173">
-        <v>10</v>
-      </c>
-      <c r="D173" s="1">
+      <c r="B173" s="7">
+        <v>3</v>
+      </c>
+      <c r="C173" s="7">
+        <v>10</v>
+      </c>
+      <c r="D173" s="6">
         <f t="shared" si="3"/>
         <v>41615</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A174" s="2">
+    <row r="174" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="6">
         <v>41637</v>
       </c>
-      <c r="C174">
-        <v>10</v>
-      </c>
-      <c r="D174" s="1">
+      <c r="B174" s="7">
+        <v>3</v>
+      </c>
+      <c r="C174" s="7">
+        <v>10</v>
+      </c>
+      <c r="D174" s="6">
         <f t="shared" si="3"/>
         <v>41622</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" s="2">
+    <row r="175" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="6">
         <v>41644</v>
       </c>
-      <c r="C175">
-        <v>10</v>
-      </c>
-      <c r="D175" s="1">
+      <c r="B175" s="7">
+        <v>3</v>
+      </c>
+      <c r="C175" s="7">
+        <v>10</v>
+      </c>
+      <c r="D175" s="6">
         <f t="shared" si="3"/>
         <v>41629</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" s="2">
+    <row r="176" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="6">
         <v>41651</v>
       </c>
-      <c r="C176">
-        <v>10</v>
-      </c>
-      <c r="D176" s="1">
+      <c r="B176" s="7">
+        <v>3</v>
+      </c>
+      <c r="C176" s="7">
+        <v>10</v>
+      </c>
+      <c r="D176" s="6">
         <f t="shared" si="3"/>
         <v>41636</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" s="2">
+    <row r="177" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="6">
         <v>41658</v>
       </c>
-      <c r="C177">
-        <v>10</v>
-      </c>
-      <c r="D177" s="1">
+      <c r="B177" s="7">
+        <v>2</v>
+      </c>
+      <c r="C177" s="7">
+        <v>10</v>
+      </c>
+      <c r="D177" s="6">
         <f t="shared" si="3"/>
         <v>41643</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" s="2">
+    <row r="178" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="6">
         <v>41665</v>
       </c>
-      <c r="C178">
-        <v>10</v>
-      </c>
-      <c r="D178" s="1">
+      <c r="B178" s="7">
+        <v>2</v>
+      </c>
+      <c r="C178" s="7">
+        <v>10</v>
+      </c>
+      <c r="D178" s="6">
         <f t="shared" si="3"/>
         <v>41650</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" s="2">
+    <row r="179" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="6">
         <v>41672</v>
       </c>
-      <c r="C179">
-        <v>10</v>
-      </c>
-      <c r="D179" s="1">
+      <c r="B179" s="7">
+        <v>2</v>
+      </c>
+      <c r="C179" s="7">
+        <v>10</v>
+      </c>
+      <c r="D179" s="6">
         <f t="shared" si="3"/>
         <v>41657</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" s="2">
+    <row r="180" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="6">
         <v>41679</v>
       </c>
-      <c r="C180">
-        <v>10</v>
-      </c>
-      <c r="D180" s="1">
+      <c r="B180" s="7">
+        <v>2</v>
+      </c>
+      <c r="C180" s="7">
+        <v>10</v>
+      </c>
+      <c r="D180" s="6">
         <f t="shared" si="3"/>
         <v>41664</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" s="2">
+    <row r="181" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="6">
         <v>41686</v>
       </c>
-      <c r="C181">
-        <v>10</v>
-      </c>
-      <c r="D181" s="1">
+      <c r="B181" s="7">
+        <v>2</v>
+      </c>
+      <c r="C181" s="7">
+        <v>10</v>
+      </c>
+      <c r="D181" s="6">
         <f t="shared" si="3"/>
         <v>41671</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" s="2">
+    <row r="182" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="6">
         <v>41693</v>
       </c>
-      <c r="C182">
-        <v>10</v>
-      </c>
-      <c r="D182" s="1">
+      <c r="B182" s="7">
+        <v>4</v>
+      </c>
+      <c r="C182" s="7">
+        <v>10</v>
+      </c>
+      <c r="D182" s="6">
         <f t="shared" si="3"/>
         <v>41678</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" s="2">
+    <row r="183" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="6">
         <v>41700</v>
       </c>
-      <c r="C183">
-        <v>10</v>
-      </c>
-      <c r="D183" s="1">
+      <c r="B183" s="7">
+        <v>4</v>
+      </c>
+      <c r="C183" s="7">
+        <v>10</v>
+      </c>
+      <c r="D183" s="6">
         <f t="shared" si="3"/>
         <v>41685</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" s="2">
+    <row r="184" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="6">
         <v>41707</v>
       </c>
-      <c r="C184">
-        <v>10</v>
-      </c>
-      <c r="D184" s="1">
+      <c r="B184" s="7">
+        <v>5</v>
+      </c>
+      <c r="C184" s="7">
+        <v>10</v>
+      </c>
+      <c r="D184" s="6">
         <f t="shared" si="3"/>
         <v>41692</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" s="2">
+    <row r="185" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="6">
         <v>41714</v>
       </c>
-      <c r="C185">
-        <v>10</v>
-      </c>
-      <c r="D185" s="1">
+      <c r="B185" s="7">
+        <v>2</v>
+      </c>
+      <c r="C185" s="7">
+        <v>10</v>
+      </c>
+      <c r="D185" s="6">
         <f t="shared" si="3"/>
         <v>41699</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" s="2">
+    <row r="186" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="6">
         <v>41721</v>
       </c>
-      <c r="C186">
-        <v>10</v>
-      </c>
-      <c r="D186" s="1">
+      <c r="B186" s="7">
+        <v>2</v>
+      </c>
+      <c r="C186" s="7">
+        <v>10</v>
+      </c>
+      <c r="D186" s="6">
         <f t="shared" si="3"/>
         <v>41706</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" s="2">
+    <row r="187" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="6">
         <v>41728</v>
       </c>
-      <c r="C187">
-        <v>10</v>
-      </c>
-      <c r="D187" s="1">
+      <c r="B187" s="7">
+        <v>2</v>
+      </c>
+      <c r="C187" s="7">
+        <v>10</v>
+      </c>
+      <c r="D187" s="6">
         <f t="shared" si="3"/>
         <v>41713</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A188" s="2">
+    <row r="188" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="6">
         <v>41735</v>
       </c>
-      <c r="C188">
-        <v>10</v>
-      </c>
-      <c r="D188" s="1">
+      <c r="B188" s="7">
+        <v>3</v>
+      </c>
+      <c r="C188" s="7">
+        <v>10</v>
+      </c>
+      <c r="D188" s="6">
         <f t="shared" si="3"/>
         <v>41720</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A189" s="2">
+    <row r="189" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="6">
         <v>41742</v>
       </c>
-      <c r="C189">
-        <v>10</v>
-      </c>
-      <c r="D189" s="1">
+      <c r="B189" s="7">
+        <v>3</v>
+      </c>
+      <c r="C189" s="7">
+        <v>10</v>
+      </c>
+      <c r="D189" s="6">
         <f t="shared" si="3"/>
         <v>41727</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A190" s="2">
+    <row r="190" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="4">
         <v>41749</v>
       </c>
-      <c r="C190">
-        <v>10</v>
-      </c>
-      <c r="D190" s="1">
+      <c r="B190" s="5">
+        <v>3</v>
+      </c>
+      <c r="C190" s="5">
+        <v>10</v>
+      </c>
+      <c r="D190" s="4">
         <f t="shared" si="3"/>
         <v>41734</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E190" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>41756</v>
       </c>
+      <c r="B191" s="3">
+        <v>3</v>
+      </c>
       <c r="C191">
         <v>10</v>
       </c>
@@ -2982,9 +3323,12 @@
         <v>41741</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>41763</v>
+      </c>
+      <c r="B192" s="3">
+        <v>4</v>
       </c>
       <c r="C192">
         <v>10</v>
@@ -2998,6 +3342,9 @@
       <c r="A193" s="2">
         <v>41770</v>
       </c>
+      <c r="B193" s="3">
+        <v>5</v>
+      </c>
       <c r="C193">
         <v>10</v>
       </c>
@@ -3010,6 +3357,9 @@
       <c r="A194" s="2">
         <v>41777</v>
       </c>
+      <c r="B194" s="3">
+        <v>4</v>
+      </c>
       <c r="C194">
         <v>10</v>
       </c>
@@ -3022,6 +3372,9 @@
       <c r="A195" s="2">
         <v>41784</v>
       </c>
+      <c r="B195" s="3">
+        <v>6</v>
+      </c>
       <c r="C195">
         <v>10</v>
       </c>
@@ -3034,6 +3387,9 @@
       <c r="A196" s="2">
         <v>41791</v>
       </c>
+      <c r="B196" s="3">
+        <v>5</v>
+      </c>
       <c r="C196">
         <v>10</v>
       </c>
@@ -3046,6 +3402,9 @@
       <c r="A197" s="2">
         <v>41798</v>
       </c>
+      <c r="B197" s="3">
+        <v>6</v>
+      </c>
       <c r="C197">
         <v>10</v>
       </c>
@@ -3058,6 +3417,9 @@
       <c r="A198" s="2">
         <v>41805</v>
       </c>
+      <c r="B198" s="3">
+        <v>7</v>
+      </c>
       <c r="C198">
         <v>10</v>
       </c>
@@ -3070,6 +3432,9 @@
       <c r="A199" s="2">
         <v>41812</v>
       </c>
+      <c r="B199" s="3">
+        <v>10</v>
+      </c>
       <c r="C199">
         <v>10</v>
       </c>
@@ -3082,6 +3447,9 @@
       <c r="A200" s="2">
         <v>41819</v>
       </c>
+      <c r="B200" s="3">
+        <v>8</v>
+      </c>
       <c r="C200">
         <v>10</v>
       </c>
@@ -3094,6 +3462,9 @@
       <c r="A201" s="2">
         <v>41826</v>
       </c>
+      <c r="B201" s="3">
+        <v>9</v>
+      </c>
       <c r="C201">
         <v>10</v>
       </c>
@@ -3106,6 +3477,9 @@
       <c r="A202" s="2">
         <v>41833</v>
       </c>
+      <c r="B202" s="3">
+        <v>9</v>
+      </c>
       <c r="C202">
         <v>10</v>
       </c>
@@ -3118,6 +3492,9 @@
       <c r="A203" s="2">
         <v>41840</v>
       </c>
+      <c r="B203" t="s">
+        <v>4</v>
+      </c>
       <c r="C203">
         <v>10</v>
       </c>
@@ -3130,6 +3507,9 @@
       <c r="A204" s="2">
         <v>41847</v>
       </c>
+      <c r="B204" t="s">
+        <v>4</v>
+      </c>
       <c r="C204">
         <v>10</v>
       </c>
@@ -3142,6 +3522,9 @@
       <c r="A205" s="2">
         <v>41854</v>
       </c>
+      <c r="B205">
+        <v>9</v>
+      </c>
       <c r="C205">
         <v>10</v>
       </c>
@@ -3154,6 +3537,9 @@
       <c r="A206" s="2">
         <v>41861</v>
       </c>
+      <c r="B206">
+        <v>10</v>
+      </c>
       <c r="C206">
         <v>10</v>
       </c>
@@ -3166,6 +3552,9 @@
       <c r="A207" s="2">
         <v>41868</v>
       </c>
+      <c r="B207">
+        <v>5</v>
+      </c>
       <c r="C207">
         <v>10</v>
       </c>
@@ -3178,6 +3567,9 @@
       <c r="A208" s="2">
         <v>41875</v>
       </c>
+      <c r="B208">
+        <v>9</v>
+      </c>
       <c r="C208">
         <v>10</v>
       </c>
@@ -3186,10 +3578,13 @@
         <v>41860</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>41882</v>
       </c>
+      <c r="B209">
+        <v>9</v>
+      </c>
       <c r="C209">
         <v>10</v>
       </c>
@@ -3198,10 +3593,13 @@
         <v>41867</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>41889</v>
       </c>
+      <c r="B210">
+        <v>9</v>
+      </c>
       <c r="C210">
         <v>10</v>
       </c>
@@ -3210,10 +3608,13 @@
         <v>41874</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
         <v>41896</v>
       </c>
+      <c r="B211" t="s">
+        <v>4</v>
+      </c>
       <c r="C211">
         <v>10</v>
       </c>
@@ -3222,10 +3623,13 @@
         <v>41881</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>41903</v>
       </c>
+      <c r="B212" t="s">
+        <v>4</v>
+      </c>
       <c r="C212">
         <v>10</v>
       </c>
@@ -3234,10 +3638,13 @@
         <v>41888</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>41910</v>
       </c>
+      <c r="B213" t="s">
+        <v>4</v>
+      </c>
       <c r="C213">
         <v>10</v>
       </c>
@@ -3246,10 +3653,13 @@
         <v>41895</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>41917</v>
       </c>
+      <c r="B214">
+        <v>10</v>
+      </c>
       <c r="C214">
         <v>10</v>
       </c>
@@ -3258,10 +3668,13 @@
         <v>41902</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>41924</v>
       </c>
+      <c r="B215" t="s">
+        <v>4</v>
+      </c>
       <c r="C215">
         <v>10</v>
       </c>
@@ -3270,10 +3683,13 @@
         <v>41909</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>41931</v>
       </c>
+      <c r="B216" t="s">
+        <v>4</v>
+      </c>
       <c r="C216">
         <v>10</v>
       </c>
@@ -3282,10 +3698,13 @@
         <v>41916</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
         <v>41938</v>
       </c>
+      <c r="B217">
+        <v>8</v>
+      </c>
       <c r="C217">
         <v>10</v>
       </c>
@@ -3294,22 +3713,28 @@
         <v>41923</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>41945</v>
       </c>
+      <c r="B218" t="s">
+        <v>4</v>
+      </c>
       <c r="C218">
         <v>10</v>
       </c>
       <c r="D218" s="1">
-        <f t="shared" ref="D218:D255" si="4">A218-15</f>
+        <f t="shared" ref="D218:D277" si="4">A218-15</f>
         <v>41930</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>41952</v>
       </c>
+      <c r="B219" t="s">
+        <v>4</v>
+      </c>
       <c r="C219">
         <v>10</v>
       </c>
@@ -3318,10 +3743,13 @@
         <v>41937</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>41959</v>
       </c>
+      <c r="B220">
+        <v>10</v>
+      </c>
       <c r="C220">
         <v>10</v>
       </c>
@@ -3330,10 +3758,13 @@
         <v>41944</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>41966</v>
       </c>
+      <c r="B221">
+        <v>8</v>
+      </c>
       <c r="C221">
         <v>10</v>
       </c>
@@ -3342,10 +3773,13 @@
         <v>41951</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>41973</v>
       </c>
+      <c r="B222">
+        <v>8</v>
+      </c>
       <c r="C222">
         <v>10</v>
       </c>
@@ -3354,226 +3788,289 @@
         <v>41958</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A223" s="2">
+    <row r="223" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="4">
         <v>41980</v>
       </c>
-      <c r="C223">
-        <v>10</v>
-      </c>
-      <c r="D223" s="1">
+      <c r="B223" s="5">
+        <v>6</v>
+      </c>
+      <c r="C223" s="5">
+        <v>10</v>
+      </c>
+      <c r="D223" s="4">
         <f t="shared" si="4"/>
         <v>41965</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" s="2">
+      <c r="E223" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="6">
         <v>41987</v>
       </c>
-      <c r="C224">
-        <v>10</v>
-      </c>
-      <c r="D224" s="1">
+      <c r="B224" s="7">
+        <v>5</v>
+      </c>
+      <c r="C224" s="7">
+        <v>10</v>
+      </c>
+      <c r="D224" s="6">
         <f t="shared" si="4"/>
         <v>41972</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" s="2">
+    <row r="225" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="6">
         <v>41994</v>
       </c>
-      <c r="C225">
-        <v>10</v>
-      </c>
-      <c r="D225" s="1">
+      <c r="B225" s="7">
+        <v>6</v>
+      </c>
+      <c r="C225" s="7">
+        <v>10</v>
+      </c>
+      <c r="D225" s="6">
         <f t="shared" si="4"/>
         <v>41979</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A226" s="2">
+    <row r="226" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="6">
         <v>42001</v>
       </c>
-      <c r="C226">
-        <v>10</v>
-      </c>
-      <c r="D226" s="1">
+      <c r="B226" s="7">
+        <v>6</v>
+      </c>
+      <c r="C226" s="7">
+        <v>10</v>
+      </c>
+      <c r="D226" s="6">
         <f t="shared" si="4"/>
         <v>41986</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A227" s="2">
+    <row r="227" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="6">
         <v>42008</v>
       </c>
-      <c r="C227">
-        <v>10</v>
-      </c>
-      <c r="D227" s="1">
+      <c r="B227" s="7">
+        <v>6</v>
+      </c>
+      <c r="C227" s="7">
+        <v>10</v>
+      </c>
+      <c r="D227" s="6">
         <f t="shared" si="4"/>
         <v>41993</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A228" s="2">
+    <row r="228" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="6">
         <v>42015</v>
       </c>
-      <c r="C228">
-        <v>10</v>
-      </c>
-      <c r="D228" s="1">
+      <c r="B228" s="7">
+        <v>6</v>
+      </c>
+      <c r="C228" s="7">
+        <v>10</v>
+      </c>
+      <c r="D228" s="6">
         <f t="shared" si="4"/>
         <v>42000</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A229" s="2">
+    <row r="229" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="6">
         <v>42022</v>
       </c>
-      <c r="C229">
-        <v>10</v>
-      </c>
-      <c r="D229" s="1">
+      <c r="B229" s="7">
+        <v>6</v>
+      </c>
+      <c r="C229" s="7">
+        <v>10</v>
+      </c>
+      <c r="D229" s="6">
         <f t="shared" si="4"/>
         <v>42007</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A230" s="2">
+    <row r="230" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="6">
         <v>42029</v>
       </c>
-      <c r="C230">
-        <v>10</v>
-      </c>
-      <c r="D230" s="1">
+      <c r="B230" s="7">
+        <v>5</v>
+      </c>
+      <c r="C230" s="7">
+        <v>10</v>
+      </c>
+      <c r="D230" s="6">
         <f t="shared" si="4"/>
         <v>42014</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A231" s="2">
+    <row r="231" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="6">
         <v>42036</v>
       </c>
-      <c r="C231">
-        <v>10</v>
-      </c>
-      <c r="D231" s="1">
+      <c r="B231" s="7">
+        <v>7</v>
+      </c>
+      <c r="C231" s="7">
+        <v>10</v>
+      </c>
+      <c r="D231" s="6">
         <f t="shared" si="4"/>
         <v>42021</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232" s="2">
+    <row r="232" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="6">
         <v>42043</v>
       </c>
-      <c r="C232">
-        <v>10</v>
-      </c>
-      <c r="D232" s="1">
+      <c r="B232" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C232" s="7">
+        <v>10</v>
+      </c>
+      <c r="D232" s="6">
         <f t="shared" si="4"/>
         <v>42028</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A233" s="2">
+    <row r="233" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="6">
         <v>42050</v>
       </c>
-      <c r="C233">
-        <v>10</v>
-      </c>
-      <c r="D233" s="1">
+      <c r="B233" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C233" s="7">
+        <v>10</v>
+      </c>
+      <c r="D233" s="6">
         <f t="shared" si="4"/>
         <v>42035</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" s="2">
+    <row r="234" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="6">
         <v>42057</v>
       </c>
-      <c r="C234">
-        <v>10</v>
-      </c>
-      <c r="D234" s="1">
+      <c r="B234" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C234" s="7">
+        <v>10</v>
+      </c>
+      <c r="D234" s="6">
         <f t="shared" si="4"/>
         <v>42042</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" s="2">
+    <row r="235" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="6">
         <v>42064</v>
       </c>
-      <c r="C235">
-        <v>10</v>
-      </c>
-      <c r="D235" s="1">
+      <c r="B235" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C235" s="7">
+        <v>10</v>
+      </c>
+      <c r="D235" s="6">
         <f t="shared" si="4"/>
         <v>42049</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="2">
+    <row r="236" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="6">
         <v>42071</v>
       </c>
-      <c r="C236">
-        <v>10</v>
-      </c>
-      <c r="D236" s="1">
+      <c r="B236" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C236" s="7">
+        <v>10</v>
+      </c>
+      <c r="D236" s="6">
         <f t="shared" si="4"/>
         <v>42056</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" s="2">
+    <row r="237" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="6">
         <v>42078</v>
       </c>
-      <c r="C237">
-        <v>10</v>
-      </c>
-      <c r="D237" s="1">
+      <c r="B237" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C237" s="7">
+        <v>10</v>
+      </c>
+      <c r="D237" s="6">
         <f t="shared" si="4"/>
         <v>42063</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A238" s="2">
+    <row r="238" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="6">
         <v>42085</v>
       </c>
-      <c r="C238">
-        <v>10</v>
-      </c>
-      <c r="D238" s="1">
+      <c r="B238" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238" s="7">
+        <v>10</v>
+      </c>
+      <c r="D238" s="6">
         <f t="shared" si="4"/>
         <v>42070</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="2">
+    <row r="239" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="6">
         <v>42092</v>
       </c>
-      <c r="C239">
-        <v>10</v>
-      </c>
-      <c r="D239" s="1">
+      <c r="B239" s="7">
+        <v>7</v>
+      </c>
+      <c r="C239" s="7">
+        <v>10</v>
+      </c>
+      <c r="D239" s="6">
         <f t="shared" si="4"/>
         <v>42077</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="2">
+    <row r="240" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="4">
         <v>42099</v>
       </c>
-      <c r="C240">
-        <v>10</v>
-      </c>
-      <c r="D240" s="1">
+      <c r="B240" s="5">
+        <v>8</v>
+      </c>
+      <c r="C240" s="5">
+        <v>10</v>
+      </c>
+      <c r="D240" s="4">
         <f t="shared" si="4"/>
         <v>42084</v>
+      </c>
+      <c r="E240" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
         <v>42106</v>
       </c>
+      <c r="B241">
+        <v>9</v>
+      </c>
       <c r="C241">
         <v>10</v>
       </c>
@@ -3586,6 +4083,9 @@
       <c r="A242" s="2">
         <v>42113</v>
       </c>
+      <c r="B242" t="s">
+        <v>4</v>
+      </c>
       <c r="C242">
         <v>10</v>
       </c>
@@ -3598,6 +4098,9 @@
       <c r="A243" s="2">
         <v>42120</v>
       </c>
+      <c r="B243" t="s">
+        <v>4</v>
+      </c>
       <c r="C243">
         <v>10</v>
       </c>
@@ -3610,6 +4113,9 @@
       <c r="A244" s="2">
         <v>42127</v>
       </c>
+      <c r="B244" t="s">
+        <v>4</v>
+      </c>
       <c r="C244">
         <v>10</v>
       </c>
@@ -3622,6 +4128,9 @@
       <c r="A245" s="2">
         <v>42134</v>
       </c>
+      <c r="B245" t="s">
+        <v>4</v>
+      </c>
       <c r="C245">
         <v>10</v>
       </c>
@@ -3634,6 +4143,9 @@
       <c r="A246" s="2">
         <v>42141</v>
       </c>
+      <c r="B246" t="s">
+        <v>4</v>
+      </c>
       <c r="C246">
         <v>10</v>
       </c>
@@ -3646,6 +4158,9 @@
       <c r="A247" s="2">
         <v>42148</v>
       </c>
+      <c r="B247" t="s">
+        <v>4</v>
+      </c>
       <c r="C247">
         <v>10</v>
       </c>
@@ -3658,6 +4173,9 @@
       <c r="A248" s="2">
         <v>42155</v>
       </c>
+      <c r="B248" t="s">
+        <v>4</v>
+      </c>
       <c r="C248">
         <v>10</v>
       </c>
@@ -3670,6 +4188,9 @@
       <c r="A249" s="2">
         <v>42162</v>
       </c>
+      <c r="B249" t="s">
+        <v>4</v>
+      </c>
       <c r="C249">
         <v>10</v>
       </c>
@@ -3682,6 +4203,9 @@
       <c r="A250" s="2">
         <v>42169</v>
       </c>
+      <c r="B250" t="s">
+        <v>4</v>
+      </c>
       <c r="C250">
         <v>10</v>
       </c>
@@ -3694,6 +4218,9 @@
       <c r="A251" s="2">
         <v>42176</v>
       </c>
+      <c r="B251" t="s">
+        <v>4</v>
+      </c>
       <c r="C251">
         <v>10</v>
       </c>
@@ -3706,6 +4233,9 @@
       <c r="A252" s="2">
         <v>42183</v>
       </c>
+      <c r="B252" t="s">
+        <v>4</v>
+      </c>
       <c r="C252">
         <v>10</v>
       </c>
@@ -3718,6 +4248,9 @@
       <c r="A253" s="2">
         <v>42190</v>
       </c>
+      <c r="B253" t="s">
+        <v>4</v>
+      </c>
       <c r="C253">
         <v>10</v>
       </c>
@@ -3730,6 +4263,9 @@
       <c r="A254" s="2">
         <v>42197</v>
       </c>
+      <c r="B254" t="s">
+        <v>4</v>
+      </c>
       <c r="C254">
         <v>10</v>
       </c>
@@ -3742,6 +4278,9 @@
       <c r="A255" s="2">
         <v>42204</v>
       </c>
+      <c r="B255" t="s">
+        <v>4</v>
+      </c>
       <c r="C255">
         <v>10</v>
       </c>
@@ -3751,7 +4290,340 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" s="2"/>
+      <c r="A256" s="2">
+        <v>42211</v>
+      </c>
+      <c r="B256" t="s">
+        <v>4</v>
+      </c>
+      <c r="C256">
+        <v>10</v>
+      </c>
+      <c r="D256" s="1">
+        <f t="shared" si="4"/>
+        <v>42196</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="2">
+        <v>42218</v>
+      </c>
+      <c r="B257" t="s">
+        <v>4</v>
+      </c>
+      <c r="C257">
+        <v>10</v>
+      </c>
+      <c r="D257" s="1">
+        <f t="shared" si="4"/>
+        <v>42203</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="2">
+        <v>42225</v>
+      </c>
+      <c r="B258" t="s">
+        <v>4</v>
+      </c>
+      <c r="C258">
+        <v>10</v>
+      </c>
+      <c r="D258" s="1">
+        <f t="shared" si="4"/>
+        <v>42210</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="2">
+        <v>42232</v>
+      </c>
+      <c r="B259" t="s">
+        <v>4</v>
+      </c>
+      <c r="C259">
+        <v>10</v>
+      </c>
+      <c r="D259" s="1">
+        <f t="shared" si="4"/>
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="2">
+        <v>42239</v>
+      </c>
+      <c r="B260" t="s">
+        <v>4</v>
+      </c>
+      <c r="C260">
+        <v>10</v>
+      </c>
+      <c r="D260" s="1">
+        <f t="shared" si="4"/>
+        <v>42224</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" s="2">
+        <v>42246</v>
+      </c>
+      <c r="B261" t="s">
+        <v>4</v>
+      </c>
+      <c r="C261">
+        <v>10</v>
+      </c>
+      <c r="D261" s="1">
+        <f t="shared" si="4"/>
+        <v>42231</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="2">
+        <v>42253</v>
+      </c>
+      <c r="B262" t="s">
+        <v>4</v>
+      </c>
+      <c r="C262">
+        <v>10</v>
+      </c>
+      <c r="D262" s="1">
+        <f t="shared" si="4"/>
+        <v>42238</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="2">
+        <v>42260</v>
+      </c>
+      <c r="B263" t="s">
+        <v>4</v>
+      </c>
+      <c r="C263">
+        <v>10</v>
+      </c>
+      <c r="D263" s="1">
+        <f t="shared" si="4"/>
+        <v>42245</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="2">
+        <v>42267</v>
+      </c>
+      <c r="B264" t="s">
+        <v>4</v>
+      </c>
+      <c r="C264">
+        <v>10</v>
+      </c>
+      <c r="D264" s="1">
+        <f t="shared" si="4"/>
+        <v>42252</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="2">
+        <v>42274</v>
+      </c>
+      <c r="B265" t="s">
+        <v>4</v>
+      </c>
+      <c r="C265">
+        <v>10</v>
+      </c>
+      <c r="D265" s="1">
+        <f t="shared" si="4"/>
+        <v>42259</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="2">
+        <v>42281</v>
+      </c>
+      <c r="B266" t="s">
+        <v>4</v>
+      </c>
+      <c r="C266">
+        <v>10</v>
+      </c>
+      <c r="D266" s="1">
+        <f t="shared" si="4"/>
+        <v>42266</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" s="2">
+        <v>42288</v>
+      </c>
+      <c r="B267" t="s">
+        <v>4</v>
+      </c>
+      <c r="C267">
+        <v>10</v>
+      </c>
+      <c r="D267" s="1">
+        <f t="shared" si="4"/>
+        <v>42273</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268" s="2">
+        <v>42295</v>
+      </c>
+      <c r="B268" t="s">
+        <v>4</v>
+      </c>
+      <c r="C268">
+        <v>10</v>
+      </c>
+      <c r="D268" s="1">
+        <f t="shared" si="4"/>
+        <v>42280</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" s="2">
+        <v>42302</v>
+      </c>
+      <c r="B269" t="s">
+        <v>4</v>
+      </c>
+      <c r="C269">
+        <v>10</v>
+      </c>
+      <c r="D269" s="1">
+        <f t="shared" si="4"/>
+        <v>42287</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270" s="2">
+        <v>42309</v>
+      </c>
+      <c r="B270" t="s">
+        <v>4</v>
+      </c>
+      <c r="C270">
+        <v>10</v>
+      </c>
+      <c r="D270" s="1">
+        <f t="shared" si="4"/>
+        <v>42294</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271" s="2">
+        <v>42316</v>
+      </c>
+      <c r="B271" t="s">
+        <v>4</v>
+      </c>
+      <c r="C271">
+        <v>10</v>
+      </c>
+      <c r="D271" s="1">
+        <f t="shared" si="4"/>
+        <v>42301</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272" s="2">
+        <v>42323</v>
+      </c>
+      <c r="B272" t="s">
+        <v>4</v>
+      </c>
+      <c r="C272">
+        <v>10</v>
+      </c>
+      <c r="D272" s="1">
+        <f t="shared" si="4"/>
+        <v>42308</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A273" s="2">
+        <v>42330</v>
+      </c>
+      <c r="B273" t="s">
+        <v>4</v>
+      </c>
+      <c r="C273">
+        <v>10</v>
+      </c>
+      <c r="D273" s="1">
+        <f t="shared" si="4"/>
+        <v>42315</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274" s="2">
+        <v>42337</v>
+      </c>
+      <c r="B274" t="s">
+        <v>4</v>
+      </c>
+      <c r="C274">
+        <v>10</v>
+      </c>
+      <c r="D274" s="1">
+        <f t="shared" si="4"/>
+        <v>42322</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="4">
+        <v>42344</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C275" s="5">
+        <v>10</v>
+      </c>
+      <c r="D275" s="4">
+        <f t="shared" si="4"/>
+        <v>42329</v>
+      </c>
+      <c r="E275" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="6">
+        <v>42351</v>
+      </c>
+      <c r="B276" s="7">
+        <v>9</v>
+      </c>
+      <c r="C276" s="7">
+        <v>10</v>
+      </c>
+      <c r="D276" s="6">
+        <f t="shared" si="4"/>
+        <v>42336</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="6">
+        <v>42358</v>
+      </c>
+      <c r="B277" s="7">
+        <v>9</v>
+      </c>
+      <c r="C277" s="7">
+        <v>10</v>
+      </c>
+      <c r="D277" s="6">
+        <f t="shared" si="4"/>
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A278" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>